<commit_message>
added expenses from 17.03.2022
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
@@ -11,8 +11,25 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>еда</t>
+  </si>
+  <si>
+    <t>вода</t>
+  </si>
+  <si>
+    <t>15.03.2022 - 14.04.2022</t>
+  </si>
+  <si>
+    <t>медицина</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -47,8 +64,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -343,14 +361,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>186.46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added expenses from 18.03.2022
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -16,18 +16,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>еда</t>
-  </si>
-  <si>
-    <t>вода</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>15.03.2022 - 14.04.2022</t>
   </si>
   <si>
-    <t>медицина</t>
+    <t>food</t>
+  </si>
+  <si>
+    <t>whater</t>
+  </si>
+  <si>
+    <t>medicine</t>
+  </si>
+  <si>
+    <t>guests</t>
   </si>
 </sst>
 </file>
@@ -361,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -375,12 +378,12 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>186.46</v>
@@ -388,7 +391,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>46</v>
@@ -400,6 +403,14 @@
       </c>
       <c r="C4">
         <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added expenses from 19.03.2022
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -367,7 +367,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -386,7 +386,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>186.46</v>
+        <v>310.95</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>

<commit_message>
added expenses from 21.03.2022
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>15.03.2022 - 14.04.2022</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>guests</t>
+  </si>
+  <si>
+    <t>internet</t>
   </si>
 </sst>
 </file>
@@ -364,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -386,7 +389,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>310.95</v>
+        <v>452.25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -394,7 +397,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -411,6 +414,14 @@
       </c>
       <c r="C5">
         <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added expenses from 29.03.2022
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -370,7 +370,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -389,7 +389,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>452.25</v>
+        <v>1107.25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -397,7 +397,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>92</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>